<commit_message>
flutter lab11 + course work + smelov lab3
</commit_message>
<xml_diff>
--- a/4 COURSE/ЗИиНИС/lab3/enc_mpr.xlsx
+++ b/4 COURSE/ЗИиНИС/lab3/enc_mpr.xlsx
@@ -23,119 +23,119 @@
     <t>Count</t>
   </si>
   <si>
-    <t>l</t>
-  </si>
-  <si>
-    <t>m</t>
-  </si>
-  <si>
-    <t>U</t>
-  </si>
-  <si>
     <t>e</t>
   </si>
   <si>
-    <t>i</t>
-  </si>
-  <si>
-    <t>o</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> </t>
-  </si>
-  <si>
-    <t>s</t>
-  </si>
-  <si>
-    <t>u</t>
-  </si>
-  <si>
-    <t>x</t>
-  </si>
-  <si>
-    <t>S</t>
-  </si>
-  <si>
-    <t>r</t>
-  </si>
-  <si>
     <t>.</t>
   </si>
   <si>
-    <t>,</t>
+    <t>g</t>
   </si>
   <si>
     <t xml:space="preserve">
 </t>
   </si>
   <si>
+    <t>M</t>
+  </si>
+  <si>
+    <t>n</t>
+  </si>
+  <si>
+    <t>l</t>
+  </si>
+  <si>
+    <t>D</t>
+  </si>
+  <si>
+    <t>s</t>
+  </si>
+  <si>
+    <t>u</t>
+  </si>
+  <si>
+    <t>t</t>
+  </si>
+  <si>
     <t>q</t>
   </si>
   <si>
-    <t>D</t>
+    <t>m</t>
+  </si>
+  <si>
+    <t>c</t>
+  </si>
+  <si>
+    <t>a</t>
+  </si>
+  <si>
+    <t>,</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>F</t>
+  </si>
+  <si>
+    <t>P</t>
+  </si>
+  <si>
+    <t>d</t>
+  </si>
+  <si>
+    <t>U</t>
+  </si>
+  <si>
+    <t>h</t>
+  </si>
+  <si>
+    <t>L</t>
+  </si>
+  <si>
+    <t>r</t>
+  </si>
+  <si>
+    <t>v</t>
+  </si>
+  <si>
+    <t>p</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
   </si>
   <si>
     <t>f</t>
   </si>
   <si>
-    <t>F</t>
-  </si>
-  <si>
-    <t>L</t>
-  </si>
-  <si>
-    <t>n</t>
-  </si>
-  <si>
-    <t>h</t>
-  </si>
-  <si>
-    <t>M</t>
-  </si>
-  <si>
-    <t>v</t>
-  </si>
-  <si>
-    <t>d</t>
+    <t>V</t>
+  </si>
+  <si>
+    <t>j</t>
+  </si>
+  <si>
+    <t>i</t>
+  </si>
+  <si>
+    <t>o</t>
   </si>
   <si>
     <t>b</t>
   </si>
   <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>I</t>
+  </si>
+  <si>
+    <t>S</t>
+  </si>
+  <si>
     <t>X</t>
   </si>
   <si>
-    <t>p</t>
-  </si>
-  <si>
-    <t>N</t>
-  </si>
-  <si>
-    <t>c</t>
-  </si>
-  <si>
-    <t>a</t>
-  </si>
-  <si>
-    <t>I</t>
-  </si>
-  <si>
-    <t>j</t>
-  </si>
-  <si>
-    <t>t</t>
-  </si>
-  <si>
-    <t>g</t>
-  </si>
-  <si>
-    <t>V</t>
-  </si>
-  <si>
-    <t>C</t>
-  </si>
-  <si>
-    <t>P</t>
+    <t>x</t>
   </si>
 </sst>
 </file>
@@ -724,7 +724,7 @@
         <v>2</v>
       </c>
       <c r="B2">
-        <v>75</v>
+        <v>181</v>
       </c>
     </row>
     <row r="3">
@@ -732,7 +732,7 @@
         <v>3</v>
       </c>
       <c r="B3">
-        <v>47</v>
+        <v>32</v>
       </c>
     </row>
     <row r="4">
@@ -740,7 +740,7 @@
         <v>4</v>
       </c>
       <c r="B4">
-        <v>1</v>
+        <v>25</v>
       </c>
     </row>
     <row r="5">
@@ -748,7 +748,7 @@
         <v>5</v>
       </c>
       <c r="B5">
-        <v>181</v>
+        <v>3</v>
       </c>
     </row>
     <row r="6">
@@ -756,7 +756,7 @@
         <v>6</v>
       </c>
       <c r="B6">
-        <v>127</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7">
@@ -764,7 +764,7 @@
         <v>7</v>
       </c>
       <c r="B7">
-        <v>64</v>
+        <v>82</v>
       </c>
     </row>
     <row r="8">
@@ -772,7 +772,7 @@
         <v>8</v>
       </c>
       <c r="B8">
-        <v>233</v>
+        <v>75</v>
       </c>
     </row>
     <row r="9">
@@ -780,7 +780,7 @@
         <v>9</v>
       </c>
       <c r="B9">
-        <v>143</v>
+        <v>3</v>
       </c>
     </row>
     <row r="10">
@@ -788,7 +788,7 @@
         <v>10</v>
       </c>
       <c r="B10">
-        <v>122</v>
+        <v>143</v>
       </c>
     </row>
     <row r="11">
@@ -796,7 +796,7 @@
         <v>11</v>
       </c>
       <c r="B11">
-        <v>3</v>
+        <v>122</v>
       </c>
     </row>
     <row r="12">
@@ -804,7 +804,7 @@
         <v>12</v>
       </c>
       <c r="B12">
-        <v>2</v>
+        <v>130</v>
       </c>
     </row>
     <row r="13">
@@ -812,7 +812,7 @@
         <v>13</v>
       </c>
       <c r="B13">
-        <v>81</v>
+        <v>9</v>
       </c>
     </row>
     <row r="14">
@@ -820,7 +820,7 @@
         <v>14</v>
       </c>
       <c r="B14">
-        <v>32</v>
+        <v>47</v>
       </c>
     </row>
     <row r="15">
@@ -828,7 +828,7 @@
         <v>15</v>
       </c>
       <c r="B15">
-        <v>19</v>
+        <v>61</v>
       </c>
     </row>
     <row r="16">
@@ -836,7 +836,7 @@
         <v>16</v>
       </c>
       <c r="B16">
-        <v>3</v>
+        <v>79</v>
       </c>
     </row>
     <row r="17">
@@ -844,7 +844,7 @@
         <v>17</v>
       </c>
       <c r="B17">
-        <v>9</v>
+        <v>19</v>
       </c>
     </row>
     <row r="18">
@@ -852,7 +852,7 @@
         <v>18</v>
       </c>
       <c r="B18">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="19">
@@ -860,7 +860,7 @@
         <v>19</v>
       </c>
       <c r="B19">
-        <v>8</v>
+        <v>3</v>
       </c>
     </row>
     <row r="20">
@@ -868,7 +868,7 @@
         <v>20</v>
       </c>
       <c r="B20">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="21">
@@ -876,7 +876,7 @@
         <v>21</v>
       </c>
       <c r="B21">
-        <v>2</v>
+        <v>49</v>
       </c>
     </row>
     <row r="22">
@@ -884,7 +884,7 @@
         <v>22</v>
       </c>
       <c r="B22">
-        <v>82</v>
+        <v>1</v>
       </c>
     </row>
     <row r="23">
@@ -900,7 +900,7 @@
         <v>24</v>
       </c>
       <c r="B24">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="25">
@@ -908,7 +908,7 @@
         <v>25</v>
       </c>
       <c r="B25">
-        <v>21</v>
+        <v>81</v>
       </c>
     </row>
     <row r="26">
@@ -916,7 +916,7 @@
         <v>26</v>
       </c>
       <c r="B26">
-        <v>49</v>
+        <v>21</v>
       </c>
     </row>
     <row r="27">
@@ -924,7 +924,7 @@
         <v>27</v>
       </c>
       <c r="B27">
-        <v>18</v>
+        <v>25</v>
       </c>
     </row>
     <row r="28">
@@ -932,7 +932,7 @@
         <v>28</v>
       </c>
       <c r="B28">
-        <v>1</v>
+        <v>233</v>
       </c>
     </row>
     <row r="29">
@@ -940,7 +940,7 @@
         <v>29</v>
       </c>
       <c r="B29">
-        <v>25</v>
+        <v>8</v>
       </c>
     </row>
     <row r="30">
@@ -948,7 +948,7 @@
         <v>30</v>
       </c>
       <c r="B30">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="31">
@@ -956,7 +956,7 @@
         <v>31</v>
       </c>
       <c r="B31">
-        <v>61</v>
+        <v>1</v>
       </c>
     </row>
     <row r="32">
@@ -964,7 +964,7 @@
         <v>32</v>
       </c>
       <c r="B32">
-        <v>79</v>
+        <v>127</v>
       </c>
     </row>
     <row r="33">
@@ -972,7 +972,7 @@
         <v>33</v>
       </c>
       <c r="B33">
-        <v>3</v>
+        <v>64</v>
       </c>
     </row>
     <row r="34">
@@ -980,7 +980,7 @@
         <v>34</v>
       </c>
       <c r="B34">
-        <v>1</v>
+        <v>18</v>
       </c>
     </row>
     <row r="35">
@@ -988,7 +988,7 @@
         <v>35</v>
       </c>
       <c r="B35">
-        <v>130</v>
+        <v>2</v>
       </c>
     </row>
     <row r="36">
@@ -996,7 +996,7 @@
         <v>36</v>
       </c>
       <c r="B36">
-        <v>25</v>
+        <v>3</v>
       </c>
     </row>
     <row r="37">
@@ -1004,7 +1004,7 @@
         <v>37</v>
       </c>
       <c r="B37">
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="38">
@@ -1012,7 +1012,7 @@
         <v>38</v>
       </c>
       <c r="B38">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="39">
@@ -1020,7 +1020,7 @@
         <v>39</v>
       </c>
       <c r="B39">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>